<commit_message>
msfo add selected loan pact
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx/msfo.xlsx
+++ b/src/main/resources/xlsx/msfo.xlsx
@@ -1857,7 +1857,19 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1868,6 +1880,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1885,45 +1924,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2612,8 +2612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="C123" sqref="C123"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4555,11 +4555,11 @@
         <v>2200</v>
       </c>
       <c r="C127" s="44">
-        <f>SUM(C123:C126)</f>
+        <f>C123-C124-C125-C126</f>
         <v>0</v>
       </c>
       <c r="D127" s="44">
-        <f>SUM(D123:D126)</f>
+        <f>D123-D124-D125-D126</f>
         <v>0</v>
       </c>
     </row>
@@ -4641,11 +4641,11 @@
         <v>2300</v>
       </c>
       <c r="C133" s="44">
-        <f>SUM(C127:C132)</f>
+        <f>C127+C128+C129-C130+C131-C132</f>
         <v>0</v>
       </c>
       <c r="D133" s="44">
-        <f>SUM(D127:D132)</f>
+        <f>D127+D128+D129-D130+D131-D132</f>
         <v>0</v>
       </c>
     </row>
@@ -4699,11 +4699,11 @@
         <v>2400</v>
       </c>
       <c r="C137" s="44">
-        <f>SUM(C133:C136)</f>
+        <f>C133-C134+C135+C136</f>
         <v>0</v>
       </c>
       <c r="D137" s="44">
-        <f>SUM(D133:D136)</f>
+        <f>D133-D134+D135+D136</f>
         <v>0</v>
       </c>
     </row>
@@ -7180,28 +7180,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="A275:A279"/>
-    <mergeCell ref="A280:A284"/>
-    <mergeCell ref="A285:A289"/>
-    <mergeCell ref="A290:A294"/>
-    <mergeCell ref="A245:A249"/>
-    <mergeCell ref="A250:A254"/>
-    <mergeCell ref="A255:A259"/>
-    <mergeCell ref="A260:A264"/>
-    <mergeCell ref="A265:A269"/>
-    <mergeCell ref="A270:A274"/>
-    <mergeCell ref="A240:A244"/>
-    <mergeCell ref="A185:A189"/>
-    <mergeCell ref="A190:A194"/>
-    <mergeCell ref="A195:A199"/>
-    <mergeCell ref="A200:A204"/>
-    <mergeCell ref="A205:A209"/>
-    <mergeCell ref="A210:A214"/>
-    <mergeCell ref="A215:A219"/>
-    <mergeCell ref="A220:A224"/>
-    <mergeCell ref="A225:A229"/>
-    <mergeCell ref="A230:A234"/>
-    <mergeCell ref="A235:A239"/>
     <mergeCell ref="A180:A184"/>
     <mergeCell ref="A140:A144"/>
     <mergeCell ref="F140:F144"/>
@@ -7218,6 +7196,28 @@
     <mergeCell ref="A170:A174"/>
     <mergeCell ref="F171:F175"/>
     <mergeCell ref="A175:A179"/>
+    <mergeCell ref="A240:A244"/>
+    <mergeCell ref="A185:A189"/>
+    <mergeCell ref="A190:A194"/>
+    <mergeCell ref="A195:A199"/>
+    <mergeCell ref="A200:A204"/>
+    <mergeCell ref="A205:A209"/>
+    <mergeCell ref="A210:A214"/>
+    <mergeCell ref="A215:A219"/>
+    <mergeCell ref="A220:A224"/>
+    <mergeCell ref="A225:A229"/>
+    <mergeCell ref="A230:A234"/>
+    <mergeCell ref="A235:A239"/>
+    <mergeCell ref="A275:A279"/>
+    <mergeCell ref="A280:A284"/>
+    <mergeCell ref="A285:A289"/>
+    <mergeCell ref="A290:A294"/>
+    <mergeCell ref="A245:A249"/>
+    <mergeCell ref="A250:A254"/>
+    <mergeCell ref="A255:A259"/>
+    <mergeCell ref="A260:A264"/>
+    <mergeCell ref="A265:A269"/>
+    <mergeCell ref="A270:A274"/>
   </mergeCells>
   <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B49">
@@ -12617,23 +12617,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A126:A130"/>
-    <mergeCell ref="A71:A75"/>
-    <mergeCell ref="A76:A80"/>
-    <mergeCell ref="A81:A85"/>
-    <mergeCell ref="A86:A90"/>
-    <mergeCell ref="A91:A95"/>
-    <mergeCell ref="A96:A100"/>
-    <mergeCell ref="A101:A105"/>
-    <mergeCell ref="A106:A110"/>
-    <mergeCell ref="A111:A115"/>
-    <mergeCell ref="A116:A120"/>
-    <mergeCell ref="A121:A125"/>
-    <mergeCell ref="A131:A135"/>
-    <mergeCell ref="A136:A140"/>
-    <mergeCell ref="A141:A145"/>
-    <mergeCell ref="A146:A150"/>
-    <mergeCell ref="A151:A155"/>
     <mergeCell ref="A201:A205"/>
     <mergeCell ref="A206:A210"/>
     <mergeCell ref="A211:A215"/>
@@ -12647,6 +12630,23 @@
     <mergeCell ref="A171:A175"/>
     <mergeCell ref="A176:A180"/>
     <mergeCell ref="A161:A165"/>
+    <mergeCell ref="A131:A135"/>
+    <mergeCell ref="A136:A140"/>
+    <mergeCell ref="A141:A145"/>
+    <mergeCell ref="A146:A150"/>
+    <mergeCell ref="A151:A155"/>
+    <mergeCell ref="A126:A130"/>
+    <mergeCell ref="A71:A75"/>
+    <mergeCell ref="A76:A80"/>
+    <mergeCell ref="A81:A85"/>
+    <mergeCell ref="A86:A90"/>
+    <mergeCell ref="A91:A95"/>
+    <mergeCell ref="A96:A100"/>
+    <mergeCell ref="A101:A105"/>
+    <mergeCell ref="A106:A110"/>
+    <mergeCell ref="A111:A115"/>
+    <mergeCell ref="A116:A120"/>
+    <mergeCell ref="A121:A125"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -14035,20 +14035,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B1" s="203" t="s">
+      <c r="B1" s="204" t="s">
         <v>206</v>
       </c>
-      <c r="C1" s="204"/>
-      <c r="P1" s="209" t="s">
+      <c r="C1" s="205"/>
+      <c r="P1" s="194" t="s">
         <v>218</v>
       </c>
-      <c r="Q1" s="210"/>
-      <c r="R1" s="211"/>
-      <c r="T1" s="212" t="s">
+      <c r="Q1" s="195"/>
+      <c r="R1" s="196"/>
+      <c r="T1" s="197" t="s">
         <v>219</v>
       </c>
-      <c r="U1" s="212"/>
-      <c r="V1" s="212"/>
+      <c r="U1" s="197"/>
+      <c r="V1" s="197"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B2" s="30" t="s">
@@ -14133,10 +14133,10 @@
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B5" s="205" t="s">
+      <c r="B5" s="206" t="s">
         <v>227</v>
       </c>
-      <c r="C5" s="206"/>
+      <c r="C5" s="207"/>
       <c r="P5" s="114" t="s">
         <v>228</v>
       </c>
@@ -14233,67 +14233,67 @@
     </row>
     <row r="10" spans="1:29" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="128"/>
-      <c r="B10" s="207" t="s">
+      <c r="B10" s="208" t="s">
         <v>234</v>
       </c>
-      <c r="C10" s="207"/>
-      <c r="D10" s="207" t="s">
+      <c r="C10" s="208"/>
+      <c r="D10" s="208" t="s">
         <v>235</v>
       </c>
-      <c r="E10" s="207"/>
-      <c r="F10" s="207" t="s">
+      <c r="E10" s="208"/>
+      <c r="F10" s="208" t="s">
         <v>236</v>
       </c>
-      <c r="G10" s="207"/>
-      <c r="H10" s="197" t="s">
+      <c r="G10" s="208"/>
+      <c r="H10" s="210" t="s">
         <v>237</v>
       </c>
-      <c r="I10" s="198"/>
-      <c r="J10" s="198"/>
-      <c r="K10" s="199"/>
-      <c r="L10" s="200" t="s">
+      <c r="I10" s="211"/>
+      <c r="J10" s="211"/>
+      <c r="K10" s="212"/>
+      <c r="L10" s="213" t="s">
         <v>238</v>
       </c>
-      <c r="M10" s="201"/>
-      <c r="N10" s="201"/>
-      <c r="O10" s="202"/>
-      <c r="P10" s="194" t="s">
+      <c r="M10" s="214"/>
+      <c r="N10" s="214"/>
+      <c r="O10" s="215"/>
+      <c r="P10" s="198" t="s">
         <v>239</v>
       </c>
-      <c r="Q10" s="194" t="s">
+      <c r="Q10" s="198" t="s">
         <v>240</v>
       </c>
-      <c r="R10" s="194" t="s">
+      <c r="R10" s="198" t="s">
         <v>241</v>
       </c>
-      <c r="S10" s="213" t="s">
+      <c r="S10" s="201" t="s">
         <v>230</v>
       </c>
-      <c r="T10" s="213" t="s">
+      <c r="T10" s="201" t="s">
         <v>232</v>
       </c>
-      <c r="U10" s="213" t="s">
+      <c r="U10" s="201" t="s">
         <v>242</v>
       </c>
-      <c r="V10" s="194" t="s">
+      <c r="V10" s="198" t="s">
         <v>243</v>
       </c>
-      <c r="W10" s="213" t="s">
+      <c r="W10" s="201" t="s">
         <v>242</v>
       </c>
-      <c r="X10" s="194" t="s">
+      <c r="X10" s="198" t="s">
         <v>243</v>
       </c>
-      <c r="Z10" s="208" t="s">
+      <c r="Z10" s="193" t="s">
         <v>279</v>
       </c>
-      <c r="AA10" s="208" t="s">
+      <c r="AA10" s="193" t="s">
         <v>280</v>
       </c>
-      <c r="AB10" s="208" t="s">
+      <c r="AB10" s="193" t="s">
         <v>279</v>
       </c>
-      <c r="AC10" s="208" t="s">
+      <c r="AC10" s="193" t="s">
         <v>280</v>
       </c>
     </row>
@@ -14333,19 +14333,19 @@
         <v>245</v>
       </c>
       <c r="O11" s="129"/>
-      <c r="P11" s="195"/>
-      <c r="Q11" s="195"/>
-      <c r="R11" s="195"/>
-      <c r="S11" s="214"/>
-      <c r="T11" s="214"/>
-      <c r="U11" s="214"/>
-      <c r="V11" s="195"/>
-      <c r="W11" s="214"/>
-      <c r="X11" s="195"/>
-      <c r="Z11" s="208"/>
-      <c r="AA11" s="208"/>
-      <c r="AB11" s="208"/>
-      <c r="AC11" s="208"/>
+      <c r="P11" s="199"/>
+      <c r="Q11" s="199"/>
+      <c r="R11" s="199"/>
+      <c r="S11" s="202"/>
+      <c r="T11" s="202"/>
+      <c r="U11" s="202"/>
+      <c r="V11" s="199"/>
+      <c r="W11" s="202"/>
+      <c r="X11" s="199"/>
+      <c r="Z11" s="193"/>
+      <c r="AA11" s="193"/>
+      <c r="AB11" s="193"/>
+      <c r="AC11" s="193"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="128"/>
@@ -14379,19 +14379,19 @@
       <c r="O12" s="130" t="s">
         <v>247</v>
       </c>
-      <c r="P12" s="196"/>
-      <c r="Q12" s="196"/>
-      <c r="R12" s="196"/>
-      <c r="S12" s="215"/>
-      <c r="T12" s="215"/>
-      <c r="U12" s="215"/>
-      <c r="V12" s="196"/>
-      <c r="W12" s="215"/>
-      <c r="X12" s="196"/>
-      <c r="Z12" s="208"/>
-      <c r="AA12" s="208"/>
-      <c r="AB12" s="208"/>
-      <c r="AC12" s="208"/>
+      <c r="P12" s="200"/>
+      <c r="Q12" s="200"/>
+      <c r="R12" s="200"/>
+      <c r="S12" s="203"/>
+      <c r="T12" s="203"/>
+      <c r="U12" s="203"/>
+      <c r="V12" s="200"/>
+      <c r="W12" s="203"/>
+      <c r="X12" s="200"/>
+      <c r="Z12" s="193"/>
+      <c r="AA12" s="193"/>
+      <c r="AB12" s="193"/>
+      <c r="AC12" s="193"/>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="131">
@@ -17155,14 +17155,14 @@
     <row r="56" spans="9:20" x14ac:dyDescent="0.25">
       <c r="I56" s="61"/>
       <c r="J56" s="61"/>
-      <c r="K56" s="193"/>
-      <c r="L56" s="193"/>
-      <c r="M56" s="193"/>
+      <c r="K56" s="209"/>
+      <c r="L56" s="209"/>
+      <c r="M56" s="209"/>
       <c r="N56" s="61"/>
       <c r="O56" s="61"/>
-      <c r="P56" s="193"/>
-      <c r="Q56" s="193"/>
-      <c r="R56" s="193"/>
+      <c r="P56" s="209"/>
+      <c r="Q56" s="209"/>
+      <c r="R56" s="209"/>
       <c r="S56" s="61"/>
       <c r="T56" s="61"/>
     </row>
@@ -17266,6 +17266,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="K56:M56"/>
+    <mergeCell ref="P56:R56"/>
+    <mergeCell ref="P10:P12"/>
+    <mergeCell ref="Q10:Q12"/>
+    <mergeCell ref="R10:R12"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="L10:O10"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
     <mergeCell ref="AC10:AC12"/>
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="T1:V1"/>
@@ -17278,18 +17290,6 @@
     <mergeCell ref="S10:S12"/>
     <mergeCell ref="T10:T12"/>
     <mergeCell ref="U10:U12"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="K56:M56"/>
-    <mergeCell ref="P56:R56"/>
-    <mergeCell ref="P10:P12"/>
-    <mergeCell ref="Q10:Q12"/>
-    <mergeCell ref="R10:R12"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="L10:O10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>